<commit_message>
Updating perf results, Removing unwanted files, Refactoring
</commit_message>
<xml_diff>
--- a/NodeNettyPrefComparison.xlsx
+++ b/NodeNettyPrefComparison.xlsx
@@ -677,31 +677,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>103.25</c:v>
+                  <c:v>214.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130.75</c:v>
+                  <c:v>223.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140.25</c:v>
+                  <c:v>228.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>143.0</c:v>
+                  <c:v>231.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150.25</c:v>
+                  <c:v>239.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>160.0</c:v>
+                  <c:v>248.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>205.0</c:v>
+                  <c:v>273.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2256.75</c:v>
+                  <c:v>1114.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3764.5</c:v>
+                  <c:v>3431.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -718,11 +718,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="3662264"/>
-        <c:axId val="3665336"/>
+        <c:axId val="541289432"/>
+        <c:axId val="571553736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="3662264"/>
+        <c:axId val="541289432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,7 +732,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3665336"/>
+        <c:crossAx val="571553736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -740,7 +740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3665336"/>
+        <c:axId val="571553736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3662264"/>
+        <c:crossAx val="541289432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -991,31 +991,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>105.5</c:v>
+                  <c:v>214.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130.0</c:v>
+                  <c:v>224.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>139.0</c:v>
+                  <c:v>230.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>141.5</c:v>
+                  <c:v>233.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>147.0</c:v>
+                  <c:v>242.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>158.0</c:v>
+                  <c:v>252.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>179.0</c:v>
+                  <c:v>277.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2360.0</c:v>
+                  <c:v>1212.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3768.5</c:v>
+                  <c:v>3433.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1032,11 +1032,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="426278888"/>
-        <c:axId val="426281960"/>
+        <c:axId val="541602056"/>
+        <c:axId val="541175144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="426278888"/>
+        <c:axId val="541602056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="426281960"/>
+        <c:crossAx val="541175144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1054,7 +1054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426281960"/>
+        <c:axId val="541175144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1065,7 +1065,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="426278888"/>
+        <c:crossAx val="541602056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1500,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2735,24 +2735,24 @@
         <v>0.5</v>
       </c>
       <c r="L36">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="M36">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="N36">
-        <v>94</v>
+        <v>219</v>
       </c>
       <c r="O36">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="P36" s="1">
         <f>AVERAGE(L36:O36)</f>
-        <v>103.25</v>
+        <v>214</v>
       </c>
       <c r="Q36" s="1">
         <f>MEDIAN(L36:O36)</f>
-        <v>105.5</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -2760,47 +2760,47 @@
         <v>1</v>
       </c>
       <c r="B37">
-        <v>4.9267500000000002</v>
+        <v>7.7141330000000004</v>
       </c>
       <c r="C37">
-        <v>4.8406849999999997</v>
+        <v>7.6513229999999997</v>
       </c>
       <c r="D37">
-        <v>4.7721629999999999</v>
+        <v>7.9017299999999997</v>
       </c>
       <c r="E37">
-        <v>4.7659690000000001</v>
+        <v>7.6940770000000001</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" ref="F37:F47" si="8">AVERAGE(B37:E37)</f>
-        <v>4.8263917499999991</v>
+        <v>7.7403157499999997</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" ref="G37:G47" si="9">MEDIAN(B37:E37)</f>
-        <v>4.8064239999999998</v>
+        <v>7.7041050000000002</v>
       </c>
       <c r="K37" s="6">
         <v>0.66</v>
       </c>
       <c r="L37">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="M37">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="N37">
-        <v>130</v>
+        <v>228</v>
       </c>
       <c r="O37">
-        <v>126</v>
+        <v>220</v>
       </c>
       <c r="P37" s="1">
         <f t="shared" ref="P37:P44" si="10">AVERAGE(L37:O37)</f>
-        <v>130.75</v>
+        <v>223.25</v>
       </c>
       <c r="Q37" s="1">
         <f t="shared" ref="Q37:Q44" si="11">MEDIAN(L37:O37)</f>
-        <v>130</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -2831,24 +2831,24 @@
         <v>0.75</v>
       </c>
       <c r="L38">
-        <v>136</v>
+        <v>219</v>
       </c>
       <c r="M38">
-        <v>141</v>
+        <v>234</v>
       </c>
       <c r="N38">
-        <v>137</v>
+        <v>234</v>
       </c>
       <c r="O38">
-        <v>147</v>
+        <v>226</v>
       </c>
       <c r="P38" s="1">
         <f t="shared" si="10"/>
-        <v>140.25</v>
+        <v>228.25</v>
       </c>
       <c r="Q38" s="1">
         <f t="shared" si="11"/>
-        <v>139</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -2856,47 +2856,47 @@
         <v>3</v>
       </c>
       <c r="B39">
-        <v>2966</v>
+        <v>27074</v>
       </c>
       <c r="C39">
-        <v>2961</v>
+        <v>2977</v>
       </c>
       <c r="D39">
-        <v>2991</v>
+        <v>3004</v>
       </c>
       <c r="E39">
-        <v>3011</v>
+        <v>2968</v>
       </c>
       <c r="F39" s="5">
         <f t="shared" si="8"/>
-        <v>2982.25</v>
+        <v>9005.75</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="9"/>
-        <v>2978.5</v>
+        <v>2990.5</v>
       </c>
       <c r="K39" s="6">
         <v>0.8</v>
       </c>
       <c r="L39">
-        <v>139</v>
+        <v>221</v>
       </c>
       <c r="M39">
-        <v>143</v>
+        <v>237</v>
       </c>
       <c r="N39">
-        <v>140</v>
+        <v>238</v>
       </c>
       <c r="O39">
-        <v>150</v>
+        <v>229</v>
       </c>
       <c r="P39" s="1">
         <f t="shared" si="10"/>
-        <v>143</v>
+        <v>231.25</v>
       </c>
       <c r="Q39" s="1">
         <f t="shared" si="11"/>
-        <v>141.5</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -2927,24 +2927,24 @@
         <v>0.9</v>
       </c>
       <c r="L40">
-        <v>148</v>
+        <v>227</v>
       </c>
       <c r="M40">
-        <v>146</v>
+        <v>248</v>
       </c>
       <c r="N40">
-        <v>145</v>
+        <v>245</v>
       </c>
       <c r="O40">
-        <v>162</v>
+        <v>239</v>
       </c>
       <c r="P40" s="1">
         <f t="shared" si="10"/>
-        <v>150.25</v>
+        <v>239.75</v>
       </c>
       <c r="Q40" s="1">
         <f t="shared" si="11"/>
-        <v>147</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -2975,24 +2975,24 @@
         <v>0.95</v>
       </c>
       <c r="L41">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="M41">
-        <v>155</v>
+        <v>256</v>
       </c>
       <c r="N41">
-        <v>158</v>
+        <v>252</v>
       </c>
       <c r="O41">
-        <v>169</v>
+        <v>252</v>
       </c>
       <c r="P41" s="1">
         <f t="shared" si="10"/>
-        <v>160</v>
+        <v>248.75</v>
       </c>
       <c r="Q41" s="1">
         <f t="shared" si="11"/>
-        <v>158</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -3000,47 +3000,47 @@
         <v>6</v>
       </c>
       <c r="B42">
-        <v>4362204</v>
+        <v>4362864</v>
       </c>
       <c r="C42">
-        <v>4362234</v>
+        <v>4362138</v>
       </c>
       <c r="D42">
-        <v>4362054</v>
+        <v>4362268</v>
       </c>
       <c r="E42">
-        <v>4361934</v>
+        <v>4362192</v>
       </c>
       <c r="F42" s="5">
         <f t="shared" si="8"/>
-        <v>4362106.5</v>
+        <v>4362365.5</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="9"/>
-        <v>4362129</v>
+        <v>4362230</v>
       </c>
       <c r="K42" s="6">
         <v>0.98</v>
       </c>
       <c r="L42">
-        <v>185</v>
+        <v>250</v>
       </c>
       <c r="M42">
-        <v>173</v>
+        <v>279</v>
       </c>
       <c r="N42">
-        <v>173</v>
+        <v>276</v>
       </c>
       <c r="O42">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="P42" s="1">
         <f t="shared" si="10"/>
-        <v>205</v>
+        <v>273</v>
       </c>
       <c r="Q42" s="1">
         <f t="shared" si="11"/>
-        <v>179</v>
+        <v>277.5</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -3048,47 +3048,47 @@
         <v>7</v>
       </c>
       <c r="B43">
-        <v>1242204</v>
+        <v>1242552</v>
       </c>
       <c r="C43">
-        <v>1242234</v>
+        <v>1242138</v>
       </c>
       <c r="D43">
-        <v>1242054</v>
+        <v>1242060</v>
       </c>
       <c r="E43">
-        <v>1241934</v>
+        <v>1242192</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="8"/>
-        <v>1242106.5</v>
+        <v>1242235.5</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="9"/>
-        <v>1242129</v>
+        <v>1242165</v>
       </c>
       <c r="K43" s="6">
         <v>0.99</v>
       </c>
       <c r="L43">
-        <v>1179</v>
+        <v>387</v>
       </c>
       <c r="M43">
-        <v>1596</v>
+        <v>1647</v>
       </c>
       <c r="N43">
-        <v>3128</v>
+        <v>1618</v>
       </c>
       <c r="O43">
-        <v>3124</v>
+        <v>807</v>
       </c>
       <c r="P43" s="1">
         <f t="shared" si="10"/>
-        <v>2256.75</v>
+        <v>1114.75</v>
       </c>
       <c r="Q43" s="1">
         <f t="shared" si="11"/>
-        <v>2360</v>
+        <v>1212.5</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -3096,47 +3096,47 @@
         <v>8</v>
       </c>
       <c r="B44">
-        <v>6089.2</v>
+        <v>3888.97</v>
       </c>
       <c r="C44">
-        <v>6197.47</v>
+        <v>3920.89</v>
       </c>
       <c r="D44">
-        <v>6286.46</v>
+        <v>3796.64</v>
       </c>
       <c r="E44">
-        <v>6294.63</v>
+        <v>3899.1</v>
       </c>
       <c r="F44" s="5">
         <f t="shared" si="8"/>
-        <v>6216.9400000000005</v>
+        <v>3876.4</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" si="9"/>
-        <v>6241.9650000000001</v>
+        <v>3894.0349999999999</v>
       </c>
       <c r="K44" s="6">
         <v>1</v>
       </c>
       <c r="L44">
-        <v>4171</v>
+        <v>3401</v>
       </c>
       <c r="M44">
-        <v>3350</v>
+        <v>3459</v>
       </c>
       <c r="N44">
-        <v>3765</v>
+        <v>3444</v>
       </c>
       <c r="O44">
-        <v>3772</v>
+        <v>3422</v>
       </c>
       <c r="P44" s="1">
         <f t="shared" si="10"/>
-        <v>3764.5</v>
+        <v>3431.5</v>
       </c>
       <c r="Q44" s="1">
         <f t="shared" si="11"/>
-        <v>3768.5</v>
+        <v>3433</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -3144,24 +3144,24 @@
         <v>11</v>
       </c>
       <c r="B45">
-        <v>164.22499999999999</v>
+        <v>257.13799999999998</v>
       </c>
       <c r="C45">
-        <v>161.35599999999999</v>
+        <v>255.04400000000001</v>
       </c>
       <c r="D45">
-        <v>159.072</v>
+        <v>263.39100000000002</v>
       </c>
       <c r="E45">
-        <v>158.86600000000001</v>
+        <v>256.46899999999999</v>
       </c>
       <c r="F45" s="5">
         <f t="shared" si="8"/>
-        <v>160.87975</v>
+        <v>258.01050000000004</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="9"/>
-        <v>160.214</v>
+        <v>256.80349999999999</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -3169,24 +3169,24 @@
         <v>10</v>
       </c>
       <c r="B46">
-        <v>0.16400000000000001</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="C46">
-        <v>0.161</v>
+        <v>0.255</v>
       </c>
       <c r="D46">
-        <v>0.159</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="E46">
-        <v>0.159</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="F46" s="5">
         <f t="shared" si="8"/>
-        <v>0.16075</v>
+        <v>0.25775000000000003</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" si="9"/>
-        <v>0.16</v>
+        <v>0.25650000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="18" thickTop="1" thickBot="1">
@@ -3194,24 +3194,24 @@
         <v>9</v>
       </c>
       <c r="B47">
-        <v>864.46</v>
+        <v>552.23</v>
       </c>
       <c r="C47">
-        <v>879.83</v>
+        <v>556.64</v>
       </c>
       <c r="D47">
-        <v>892.47</v>
+        <v>539.12</v>
       </c>
       <c r="E47">
-        <v>893.63</v>
+        <v>553.54</v>
       </c>
       <c r="F47" s="5">
         <f t="shared" si="8"/>
-        <v>882.59750000000008</v>
+        <v>550.38249999999994</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="9"/>
-        <v>886.15000000000009</v>
+        <v>552.88499999999999</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="16" thickTop="1"/>

</xml_diff>